<commit_message>
added list of files
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Files_Check_List" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="194">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -373,12 +374,263 @@
   <si>
     <t xml:space="preserve">Is there commented out code (for testing) that should be removed? </t>
   </si>
+  <si>
+    <t>binary_model.c</t>
+  </si>
+  <si>
+    <t>binary_model.h</t>
+  </si>
+  <si>
+    <t>CAREL_GLOBAL_DEF.h</t>
+  </si>
+  <si>
+    <t>CBOR_CAREL.c</t>
+  </si>
+  <si>
+    <t>CBOR_CAREL.h</t>
+  </si>
+  <si>
+    <t>CMakeLists.txt</t>
+  </si>
+  <si>
+    <t>common.h</t>
+  </si>
+  <si>
+    <t>component.mk</t>
+  </si>
+  <si>
+    <t>data_types_CAREL.h</t>
+  </si>
+  <si>
+    <t>data_types_IS.h</t>
+  </si>
+  <si>
+    <t>File_System_CAREL.c</t>
+  </si>
+  <si>
+    <t>File_System_CAREL.h</t>
+  </si>
+  <si>
+    <t>File_System_IS.c</t>
+  </si>
+  <si>
+    <t>File_System_IS.h</t>
+  </si>
+  <si>
+    <t>gme_config.h</t>
+  </si>
+  <si>
+    <t>gme_types.h</t>
+  </si>
+  <si>
+    <t>GSM_Miscellaneous_IS.c</t>
+  </si>
+  <si>
+    <t>GSM_Miscellaneous_IS.h</t>
+  </si>
+  <si>
+    <t>https_client_CAREL.c</t>
+  </si>
+  <si>
+    <t>https_client_CAREL.h</t>
+  </si>
+  <si>
+    <t>https_client_IS.c</t>
+  </si>
+  <si>
+    <t>https_client_IS.h</t>
+  </si>
+  <si>
+    <t>http_server_CAREL.c</t>
+  </si>
+  <si>
+    <t>http_server_CAREL.h</t>
+  </si>
+  <si>
+    <t>http_server_IS.c</t>
+  </si>
+  <si>
+    <t>http_server_IS.h</t>
+  </si>
+  <si>
+    <t>IO_Port_IS.c</t>
+  </si>
+  <si>
+    <t>IO_Port_IS.h</t>
+  </si>
+  <si>
+    <t>Kconfig.projbuild</t>
+  </si>
+  <si>
+    <t>Led_Manager_IS.c</t>
+  </si>
+  <si>
+    <t>Led_Manager_IS.h</t>
+  </si>
+  <si>
+    <t>lista.txt</t>
+  </si>
+  <si>
+    <t>main_CAREL.c</t>
+  </si>
+  <si>
+    <t>main_CAREL.h</t>
+  </si>
+  <si>
+    <t>main_IS.c</t>
+  </si>
+  <si>
+    <t>main_IS.h</t>
+  </si>
+  <si>
+    <t>Miscellaneous_IS.h</t>
+  </si>
+  <si>
+    <t>mobile.c</t>
+  </si>
+  <si>
+    <t>mobile.h</t>
+  </si>
+  <si>
+    <t>modbus_IS.c</t>
+  </si>
+  <si>
+    <t>modbus_IS.h</t>
+  </si>
+  <si>
+    <t>MQTT_Interface_CAREL.c</t>
+  </si>
+  <si>
+    <t>MQTT_Interface_CAREL.h</t>
+  </si>
+  <si>
+    <t>MQTT_Interface_IS.c</t>
+  </si>
+  <si>
+    <t>MQTT_Interface_IS.h</t>
+  </si>
+  <si>
+    <t>nvm_CAREL.c</t>
+  </si>
+  <si>
+    <t>nvm_CAREL.h</t>
+  </si>
+  <si>
+    <t>nvm_IS.c</t>
+  </si>
+  <si>
+    <t>nvm_IS.h</t>
+  </si>
+  <si>
+    <t>ota_CAREL.c</t>
+  </si>
+  <si>
+    <t>ota_CAREL.h</t>
+  </si>
+  <si>
+    <t>ota_IS.c</t>
+  </si>
+  <si>
+    <t>ota_IS.h</t>
+  </si>
+  <si>
+    <t>polling_CAREL.c</t>
+  </si>
+  <si>
+    <t>polling_CAREL.h</t>
+  </si>
+  <si>
+    <t>polling_IS.c</t>
+  </si>
+  <si>
+    <t>polling_IS.h</t>
+  </si>
+  <si>
+    <t>radio.c</t>
+  </si>
+  <si>
+    <t>radio.h</t>
+  </si>
+  <si>
+    <t>RTC_IS.c</t>
+  </si>
+  <si>
+    <t>RTC_IS.h</t>
+  </si>
+  <si>
+    <t>SoftWDT.c</t>
+  </si>
+  <si>
+    <t>SoftWDT.h</t>
+  </si>
+  <si>
+    <t>sys_CAREL.c</t>
+  </si>
+  <si>
+    <t>sys_CAREL.h</t>
+  </si>
+  <si>
+    <t>sys_IS.c</t>
+  </si>
+  <si>
+    <t>sys_IS.h</t>
+  </si>
+  <si>
+    <t>test_hw_CAREL.c</t>
+  </si>
+  <si>
+    <t>test_hw_CAREL.h</t>
+  </si>
+  <si>
+    <t>tinycbor</t>
+  </si>
+  <si>
+    <t>types.h</t>
+  </si>
+  <si>
+    <t>utilities_CAREL.c</t>
+  </si>
+  <si>
+    <t>utilities_CAREL.h</t>
+  </si>
+  <si>
+    <t>wifi.c</t>
+  </si>
+  <si>
+    <t>wifi.h</t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Revided 
+Assigned to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link to Excel revision 
+file </t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Chiebao</t>
+  </si>
+  <si>
+    <t>Bilato</t>
+  </si>
+  <si>
+    <t>Cellini</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -407,6 +659,18 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="SimSun"/>
     </font>
   </fonts>
   <fills count="3">
@@ -757,10 +1021,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -797,17 +1062,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -819,8 +1073,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1145,15 +1416,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6267,7 +6538,7 @@
   </sheetPr>
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -6291,18 +6562,18 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
-      <c r="A2" s="39"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="26" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="9"/>
@@ -6311,7 +6582,7 @@
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
-      <c r="A4" s="39"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="13" t="s">
         <v>57</v>
       </c>
@@ -6321,8 +6592,8 @@
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="32" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="27" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -6339,8 +6610,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="12"/>
@@ -6349,10 +6620,10 @@
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A7" s="39">
+      <c r="A7" s="34">
         <v>1</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="12"/>
@@ -6361,11 +6632,11 @@
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A8" s="39">
+      <c r="A8" s="34">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="12"/>
@@ -6374,11 +6645,11 @@
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A9" s="39">
+      <c r="A9" s="34">
         <f t="shared" ref="A9:A14" si="0">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="29" t="s">
         <v>66</v>
       </c>
       <c r="C9" s="12"/>
@@ -6387,11 +6658,11 @@
       <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A10" s="39">
+      <c r="A10" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="12"/>
@@ -6400,11 +6671,11 @@
       <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A11" s="39">
+      <c r="A11" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="30" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="25"/>
@@ -6413,11 +6684,11 @@
       <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A12" s="39">
+      <c r="A12" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C12" s="12"/>
@@ -6426,11 +6697,11 @@
       <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A13" s="39">
+      <c r="A13" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="29" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="12"/>
@@ -6439,11 +6710,11 @@
       <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A14" s="39">
+      <c r="A14" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="30" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="12"/>
@@ -6452,8 +6723,8 @@
       <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="12"/>
@@ -6462,10 +6733,10 @@
       <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A16" s="39">
+      <c r="A16" s="34">
         <v>1</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C16" s="12"/>
@@ -6474,11 +6745,11 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A17" s="39">
+      <c r="A17" s="34">
         <f>A16+1</f>
         <v>2</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="12"/>
@@ -6487,11 +6758,11 @@
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A18" s="39">
+      <c r="A18" s="34">
         <f t="shared" ref="A18:A24" si="1">A17+1</f>
         <v>3</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="29" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="12"/>
@@ -6500,11 +6771,11 @@
       <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A19" s="39">
+      <c r="A19" s="34">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="29" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="12"/>
@@ -6513,11 +6784,11 @@
       <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A20" s="39">
+      <c r="A20" s="34">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="29" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="12"/>
@@ -6526,11 +6797,11 @@
       <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A21" s="39">
+      <c r="A21" s="34">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="29" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="12"/>
@@ -6539,11 +6810,11 @@
       <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A22" s="39">
+      <c r="A22" s="34">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="30" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="12"/>
@@ -6552,11 +6823,11 @@
       <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A23" s="39">
+      <c r="A23" s="34">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C23" s="12"/>
@@ -6565,11 +6836,11 @@
       <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A24" s="39">
+      <c r="A24" s="34">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="29" t="s">
         <v>80</v>
       </c>
       <c r="C24" s="12"/>
@@ -6578,8 +6849,8 @@
       <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A25" s="39"/>
-      <c r="B25" s="33" t="s">
+      <c r="A25" s="34"/>
+      <c r="B25" s="28" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="12"/>
@@ -6588,10 +6859,10 @@
       <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A26" s="39">
+      <c r="A26" s="34">
         <v>1</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="29" t="s">
         <v>81</v>
       </c>
       <c r="C26" s="12"/>
@@ -6600,11 +6871,11 @@
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A27" s="39">
+      <c r="A27" s="34">
         <f>A26+1</f>
         <v>2</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="29" t="s">
         <v>82</v>
       </c>
       <c r="C27" s="12"/>
@@ -6613,11 +6884,11 @@
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A28" s="39">
+      <c r="A28" s="34">
         <f t="shared" ref="A28:A32" si="2">A27+1</f>
         <v>3</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="29" t="s">
         <v>83</v>
       </c>
       <c r="C28" s="12"/>
@@ -6626,11 +6897,11 @@
       <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" ht="14.4">
-      <c r="A29" s="39">
+      <c r="A29" s="34">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="30" t="s">
         <v>84</v>
       </c>
       <c r="C29" s="12"/>
@@ -6639,11 +6910,11 @@
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" ht="28.8">
-      <c r="A30" s="39">
+      <c r="A30" s="34">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="30" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="12"/>
@@ -6652,11 +6923,11 @@
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" ht="28.8">
-      <c r="A31" s="39">
+      <c r="A31" s="34">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="30" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="12"/>
@@ -6665,11 +6936,11 @@
       <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" ht="14.4">
-      <c r="A32" s="39">
+      <c r="A32" s="34">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="30" t="s">
         <v>87</v>
       </c>
       <c r="C32" s="12"/>
@@ -6678,8 +6949,8 @@
       <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A33" s="39"/>
-      <c r="B33" s="33" t="s">
+      <c r="A33" s="34"/>
+      <c r="B33" s="28" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="12"/>
@@ -6688,10 +6959,10 @@
       <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A34" s="39">
+      <c r="A34" s="34">
         <v>1</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="29" t="s">
         <v>88</v>
       </c>
       <c r="C34" s="12"/>
@@ -6700,11 +6971,11 @@
       <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A35" s="39">
+      <c r="A35" s="34">
         <f>A34+1</f>
         <v>2</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="29" t="s">
         <v>89</v>
       </c>
       <c r="C35" s="20"/>
@@ -6713,11 +6984,11 @@
       <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A36" s="39">
+      <c r="A36" s="34">
         <f t="shared" ref="A36:A41" si="3">A35+1</f>
         <v>3</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="29" t="s">
         <v>90</v>
       </c>
       <c r="C36" s="20"/>
@@ -6726,11 +6997,11 @@
       <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A37" s="39">
+      <c r="A37" s="34">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="29" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="12"/>
@@ -6739,11 +7010,11 @@
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A38" s="39">
+      <c r="A38" s="34">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="29" t="s">
         <v>92</v>
       </c>
       <c r="C38" s="12"/>
@@ -6752,11 +7023,11 @@
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A39" s="39">
+      <c r="A39" s="34">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="29" t="s">
         <v>93</v>
       </c>
       <c r="C39" s="12"/>
@@ -6765,11 +7036,11 @@
       <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A40" s="39">
+      <c r="A40" s="34">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="29" t="s">
         <v>94</v>
       </c>
       <c r="C40" s="20"/>
@@ -6778,11 +7049,11 @@
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A41" s="39">
+      <c r="A41" s="34">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="29" t="s">
         <v>95</v>
       </c>
       <c r="C41" s="20"/>
@@ -6791,8 +7062,8 @@
       <c r="F41" s="19"/>
     </row>
     <row r="42" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A42" s="39"/>
-      <c r="B42" s="33" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="12"/>
@@ -6801,10 +7072,10 @@
       <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A43" s="39">
+      <c r="A43" s="34">
         <v>1</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="29" t="s">
         <v>96</v>
       </c>
       <c r="C43" s="12"/>
@@ -6813,11 +7084,11 @@
       <c r="F43" s="19"/>
     </row>
     <row r="44" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A44" s="39">
+      <c r="A44" s="34">
         <f>A43+1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="29" t="s">
         <v>97</v>
       </c>
       <c r="C44" s="12"/>
@@ -6826,11 +7097,11 @@
       <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A45" s="39">
+      <c r="A45" s="34">
         <f t="shared" ref="A45:A48" si="4">A44+1</f>
         <v>3</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="29" t="s">
         <v>98</v>
       </c>
       <c r="C45" s="12"/>
@@ -6839,11 +7110,11 @@
       <c r="F45" s="19"/>
     </row>
     <row r="46" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A46" s="39">
+      <c r="A46" s="34">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="29" t="s">
         <v>99</v>
       </c>
       <c r="C46" s="12"/>
@@ -6852,11 +7123,11 @@
       <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A47" s="39">
+      <c r="A47" s="34">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="29" t="s">
         <v>100</v>
       </c>
       <c r="C47" s="12"/>
@@ -6865,11 +7136,11 @@
       <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A48" s="39">
+      <c r="A48" s="34">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="29" t="s">
         <v>101</v>
       </c>
       <c r="C48" s="12"/>
@@ -6878,8 +7149,8 @@
       <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A49" s="39"/>
-      <c r="B49" s="33" t="s">
+      <c r="A49" s="34"/>
+      <c r="B49" s="28" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="12"/>
@@ -6888,10 +7159,10 @@
       <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A50" s="39">
+      <c r="A50" s="34">
         <v>1</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="29" t="s">
         <v>102</v>
       </c>
       <c r="C50" s="12"/>
@@ -6900,11 +7171,11 @@
       <c r="F50" s="19"/>
     </row>
     <row r="51" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A51" s="39">
+      <c r="A51" s="34">
         <f>A50+1</f>
         <v>2</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="29" t="s">
         <v>103</v>
       </c>
       <c r="C51" s="12"/>
@@ -6913,11 +7184,11 @@
       <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A52" s="39">
+      <c r="A52" s="34">
         <f t="shared" ref="A52:A58" si="5">A51+1</f>
         <v>3</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="29" t="s">
         <v>104</v>
       </c>
       <c r="C52" s="12"/>
@@ -6926,11 +7197,11 @@
       <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A53" s="39">
+      <c r="A53" s="34">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="29" t="s">
         <v>105</v>
       </c>
       <c r="C53" s="12"/>
@@ -6939,11 +7210,11 @@
       <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A54" s="39">
+      <c r="A54" s="34">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="29" t="s">
         <v>106</v>
       </c>
       <c r="C54" s="12"/>
@@ -6952,11 +7223,11 @@
       <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A55" s="39">
+      <c r="A55" s="34">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="29" t="s">
         <v>107</v>
       </c>
       <c r="C55" s="12"/>
@@ -6965,11 +7236,11 @@
       <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A56" s="39">
+      <c r="A56" s="34">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="29" t="s">
         <v>108</v>
       </c>
       <c r="C56" s="12"/>
@@ -6978,11 +7249,11 @@
       <c r="F56" s="19"/>
     </row>
     <row r="57" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A57" s="39">
+      <c r="A57" s="34">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="29" t="s">
         <v>109</v>
       </c>
       <c r="C57" s="20"/>
@@ -6991,11 +7262,11 @@
       <c r="F57" s="19"/>
     </row>
     <row r="58" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A58" s="39">
+      <c r="A58" s="34">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="31" t="s">
         <v>110</v>
       </c>
       <c r="C58" s="12"/>
@@ -7004,160 +7275,160 @@
       <c r="F58" s="19"/>
     </row>
     <row r="59" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A59" s="39"/>
-      <c r="B59" s="36"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="12"/>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
       <c r="F59" s="19"/>
     </row>
     <row r="60" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A60" s="39"/>
-      <c r="B60" s="36"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="12"/>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
       <c r="F60" s="19"/>
     </row>
     <row r="61" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A61" s="39"/>
-      <c r="B61" s="36"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="12"/>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
       <c r="F61" s="19"/>
     </row>
     <row r="62" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A62" s="39"/>
-      <c r="B62" s="36"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="31"/>
       <c r="C62" s="12"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
       <c r="F62" s="19"/>
     </row>
     <row r="63" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A63" s="39"/>
-      <c r="B63" s="36"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="12"/>
       <c r="D63" s="17"/>
       <c r="E63" s="17"/>
       <c r="F63" s="19"/>
     </row>
     <row r="64" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A64" s="39"/>
-      <c r="B64" s="36"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="12"/>
       <c r="D64" s="17"/>
       <c r="E64" s="17"/>
       <c r="F64" s="19"/>
     </row>
     <row r="65" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A65" s="39"/>
-      <c r="B65" s="36"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="12"/>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
       <c r="F65" s="19"/>
     </row>
     <row r="66" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A66" s="39"/>
-      <c r="B66" s="36"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="12"/>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
       <c r="F66" s="19"/>
     </row>
     <row r="67" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A67" s="39"/>
-      <c r="B67" s="36"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="12"/>
       <c r="D67" s="17"/>
       <c r="E67" s="17"/>
       <c r="F67" s="19"/>
     </row>
     <row r="68" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A68" s="39"/>
-      <c r="B68" s="36"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="12"/>
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
       <c r="F68" s="19"/>
     </row>
     <row r="69" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A69" s="39"/>
-      <c r="B69" s="37"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="32"/>
       <c r="C69" s="12"/>
       <c r="D69" s="17"/>
       <c r="E69" s="17"/>
       <c r="F69" s="19"/>
     </row>
     <row r="70" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A70" s="39"/>
-      <c r="B70" s="37"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="32"/>
       <c r="C70" s="12"/>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
       <c r="F70" s="19"/>
     </row>
     <row r="71" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A71" s="39"/>
-      <c r="B71" s="37"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="32"/>
       <c r="C71" s="21"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="19"/>
     </row>
     <row r="72" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A72" s="39"/>
-      <c r="B72" s="37"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="32"/>
       <c r="C72" s="12"/>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
       <c r="F72" s="19"/>
     </row>
     <row r="73" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A73" s="39"/>
-      <c r="B73" s="37"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="32"/>
       <c r="C73" s="21"/>
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
       <c r="F73" s="19"/>
     </row>
     <row r="74" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A74" s="39"/>
-      <c r="B74" s="37"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="32"/>
       <c r="C74" s="12"/>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
       <c r="F74" s="19"/>
     </row>
     <row r="75" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A75" s="39"/>
-      <c r="B75" s="37"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="32"/>
       <c r="C75" s="12"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="19"/>
     </row>
     <row r="76" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A76" s="39"/>
-      <c r="B76" s="37"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="32"/>
       <c r="C76" s="21"/>
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
       <c r="F76" s="19"/>
     </row>
     <row r="77" spans="1:6" ht="13.65" customHeight="1">
-      <c r="A77" s="39"/>
-      <c r="B77" s="37"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="32"/>
       <c r="C77" s="21"/>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
       <c r="F77" s="19"/>
     </row>
     <row r="78" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
-      <c r="A78" s="39"/>
-      <c r="B78" s="38"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="33"/>
       <c r="C78" s="22"/>
       <c r="D78" s="23"/>
       <c r="E78" s="23"/>
@@ -14531,4 +14802,872 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="74.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="43.2">
+      <c r="A1" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>167</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>173</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>174</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>184</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some inspection plan check files
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="197">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -624,6 +624,15 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_CBOR_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_data_types_CAREL_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1073,6 +1082,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1084,11 +1097,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -1416,15 +1426,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6563,13 +6573,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="36"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14810,7 +14820,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14821,17 +14831,17 @@
     <col min="4" max="4" width="74.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:4" ht="28.8">
+      <c r="A1" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="36" t="s">
         <v>188</v>
       </c>
     </row>
@@ -14859,6 +14869,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14881,6 +14892,9 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D5" s="42" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
@@ -14892,6 +14906,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14936,6 +14951,9 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D10" s="42" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
@@ -14947,6 +14965,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14958,6 +14977,9 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D12" s="42" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
@@ -14969,6 +14991,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15664,10 +15687,19 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D10:D11" r:id="rId3" display="C780_PT15_FW_Code_Inspection_Plan_data_types_CAREL_IS.xlsx"/>
+    <hyperlink ref="D12:D13" r:id="rId4" display="C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inspection plan for led manager
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" activeTab="2"/>
+    <workbookView xWindow="1452" yWindow="2784" windowWidth="46296" windowHeight="13296" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
     <sheet name="Files_Check_List" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="198">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -633,6 +628,9 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_Led_manager.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1086,6 +1084,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1160,7 +1159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1195,7 +1194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1426,15 +1425,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6573,13 +6572,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14819,8 +14818,8 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12:D13"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14855,7 +14854,7 @@
       <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="43" t="s">
         <v>193</v>
       </c>
     </row>
@@ -14869,7 +14868,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14892,7 +14891,7 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="43" t="s">
         <v>194</v>
       </c>
     </row>
@@ -14906,7 +14905,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="43"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14951,7 +14950,7 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="43" t="s">
         <v>195</v>
       </c>
     </row>
@@ -14965,7 +14964,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="42"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14977,7 +14976,7 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="43" t="s">
         <v>196</v>
       </c>
     </row>
@@ -14991,7 +14990,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="43"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15026,7 +15025,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -15037,7 +15036,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -15048,7 +15047,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -15059,7 +15058,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -15070,7 +15069,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -15081,7 +15080,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -15092,7 +15091,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -15103,7 +15102,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -15114,7 +15113,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -15125,7 +15124,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -15136,7 +15135,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -15147,7 +15146,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -15158,7 +15157,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -15169,7 +15168,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -15180,7 +15179,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -15190,8 +15189,11 @@
       <c r="C31" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -15698,8 +15700,9 @@
     <hyperlink ref="D5" r:id="rId2"/>
     <hyperlink ref="D10:D11" r:id="rId3" display="C780_PT15_FW_Code_Inspection_Plan_data_types_CAREL_IS.xlsx"/>
     <hyperlink ref="D12:D13" r:id="rId4" display="C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx"/>
+    <hyperlink ref="D31" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
main_CAREL/main_IS checked with inspection plan
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="200">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -631,6 +631,12 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_Led_manager.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_main_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_main_IS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1084,6 +1090,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1425,15 +1432,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6572,13 +6579,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14818,8 +14825,8 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14854,7 +14861,7 @@
       <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="44" t="s">
         <v>193</v>
       </c>
     </row>
@@ -14868,7 +14875,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="45"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14891,7 +14898,7 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="44" t="s">
         <v>194</v>
       </c>
     </row>
@@ -14905,7 +14912,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="45"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14950,7 +14957,7 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="44" t="s">
         <v>195</v>
       </c>
     </row>
@@ -14964,7 +14971,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14976,7 +14983,7 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="44" t="s">
         <v>196</v>
       </c>
     </row>
@@ -14990,7 +14997,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="43"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15204,7 +15211,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -15215,7 +15222,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -15225,8 +15232,11 @@
       <c r="C34" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -15237,7 +15247,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -15247,8 +15257,11 @@
       <c r="C36" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -15259,7 +15272,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -15270,7 +15283,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -15281,7 +15294,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -15292,7 +15305,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -15303,7 +15316,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -15314,7 +15327,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -15325,7 +15338,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -15336,7 +15349,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -15347,7 +15360,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -15358,7 +15371,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -15369,7 +15382,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -15701,8 +15714,10 @@
     <hyperlink ref="D10:D11" r:id="rId3" display="C780_PT15_FW_Code_Inspection_Plan_data_types_CAREL_IS.xlsx"/>
     <hyperlink ref="D12:D13" r:id="rId4" display="C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx"/>
     <hyperlink ref="D31" r:id="rId5"/>
+    <hyperlink ref="D34" r:id="rId6"/>
+    <hyperlink ref="D36" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inspection plan MQTT_Interface_CAREL.c/.h MQTT_Interface_IS.c/.h
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -1038,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1092,6 +1092,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1432,15 +1433,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6579,13 +6580,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14825,8 +14826,8 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14861,7 +14862,7 @@
       <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>193</v>
       </c>
     </row>
@@ -14875,7 +14876,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14898,7 +14899,7 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="45" t="s">
         <v>194</v>
       </c>
     </row>
@@ -14912,7 +14913,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="46"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14957,7 +14958,7 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="45" t="s">
         <v>195</v>
       </c>
     </row>
@@ -14971,7 +14972,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14983,7 +14984,7 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="45" t="s">
         <v>196</v>
       </c>
     </row>
@@ -14997,7 +14998,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="44"/>
+      <c r="D13" s="45"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15467,7 +15468,7 @@
         <v>164</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -15477,8 +15478,8 @@
       <c r="B56" t="s">
         <v>165</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>192</v>
+      <c r="C56" s="39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -15488,8 +15489,8 @@
       <c r="B57" t="s">
         <v>166</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>192</v>
+      <c r="C57" s="39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -15499,8 +15500,8 @@
       <c r="B58" t="s">
         <v>167</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>192</v>
+      <c r="C58" s="39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:3">

</xml_diff>

<commit_message>
inspection plan Modbus_IS.c/.h polling_IS.c/.h polling_CAREL.c/.h
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="2784" windowWidth="46296" windowHeight="13296" activeTab="2"/>
+    <workbookView xWindow="1848" yWindow="3600" windowWidth="52056" windowHeight="16452" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="204">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_main_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_Modbus_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_MQTT_Interface_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_polling_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_polling_CAREL.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1050,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1093,6 +1105,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1433,15 +1447,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
+      <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6580,13 +6594,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14826,8 +14840,8 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14862,7 +14876,7 @@
       <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="47" t="s">
         <v>193</v>
       </c>
     </row>
@@ -14876,7 +14890,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14899,7 +14913,7 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="47" t="s">
         <v>194</v>
       </c>
     </row>
@@ -14913,7 +14927,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="48"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14958,7 +14972,7 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="47" t="s">
         <v>195</v>
       </c>
     </row>
@@ -14972,7 +14986,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14984,7 +14998,7 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="47" t="s">
         <v>196</v>
       </c>
     </row>
@@ -14998,7 +15012,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="45"/>
+      <c r="D13" s="47"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15316,6 +15330,9 @@
       <c r="C41" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D41" s="40" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
@@ -15338,6 +15355,9 @@
       <c r="C43" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D43" s="40" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
@@ -15360,6 +15380,9 @@
       <c r="C45" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D45" s="40" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
@@ -15394,7 +15417,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -15405,7 +15428,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -15416,7 +15439,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -15427,7 +15450,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -15438,7 +15461,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -15449,7 +15472,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -15460,7 +15483,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -15470,8 +15493,11 @@
       <c r="C55" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -15482,7 +15508,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -15492,8 +15518,11 @@
       <c r="C57" s="39" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -15504,7 +15533,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -15515,7 +15544,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -15526,7 +15555,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -15537,7 +15566,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -15548,7 +15577,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -15559,7 +15588,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -15717,8 +15746,13 @@
     <hyperlink ref="D31" r:id="rId5"/>
     <hyperlink ref="D34" r:id="rId6"/>
     <hyperlink ref="D36" r:id="rId7"/>
+    <hyperlink ref="D41" r:id="rId8"/>
+    <hyperlink ref="D43" r:id="rId9"/>
+    <hyperlink ref="D45" r:id="rId10"/>
+    <hyperlink ref="D55" r:id="rId11"/>
+    <hyperlink ref="D57" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inspection plan nvm_IS.c/.h nvm_CAREL.c/.h
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="3600" windowWidth="52056" windowHeight="16452" activeTab="2"/>
+    <workbookView xWindow="1848" yWindow="3600" windowWidth="46296" windowHeight="13296" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="206">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_polling_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1102,11 +1108,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1118,6 +1120,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -1447,15 +1455,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6594,13 +6602,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14840,8 +14848,8 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14876,7 +14884,7 @@
       <c r="C2" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="45" t="s">
         <v>193</v>
       </c>
     </row>
@@ -14890,7 +14898,7 @@
       <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -14913,7 +14921,7 @@
       <c r="C5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="45" t="s">
         <v>194</v>
       </c>
     </row>
@@ -14927,7 +14935,7 @@
       <c r="C6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="46"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -14972,7 +14980,7 @@
       <c r="C10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="45" t="s">
         <v>195</v>
       </c>
     </row>
@@ -14986,7 +14994,7 @@
       <c r="C11" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -14998,7 +15006,7 @@
       <c r="C12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="45" t="s">
         <v>196</v>
       </c>
     </row>
@@ -15012,7 +15020,7 @@
       <c r="C13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="45"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
@@ -15211,7 +15219,7 @@
       <c r="C31" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="44" t="s">
         <v>197</v>
       </c>
     </row>
@@ -15225,6 +15233,7 @@
       <c r="C32" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D32" s="44"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
@@ -15247,7 +15256,7 @@
       <c r="C34" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="43" t="s">
         <v>198</v>
       </c>
     </row>
@@ -15261,6 +15270,7 @@
       <c r="C35" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D35" s="43"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
@@ -15272,7 +15282,7 @@
       <c r="C36" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="43" t="s">
         <v>199</v>
       </c>
     </row>
@@ -15286,6 +15296,7 @@
       <c r="C37" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D37" s="43"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
@@ -15330,7 +15341,7 @@
       <c r="C41" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="43" t="s">
         <v>200</v>
       </c>
     </row>
@@ -15344,6 +15355,7 @@
       <c r="C42" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D42" s="43"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
@@ -15355,7 +15367,7 @@
       <c r="C43" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="43" t="s">
         <v>201</v>
       </c>
     </row>
@@ -15369,6 +15381,7 @@
       <c r="C44" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D44" s="43"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
@@ -15380,7 +15393,7 @@
       <c r="C45" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="43" t="s">
         <v>202</v>
       </c>
     </row>
@@ -15394,6 +15407,7 @@
       <c r="C46" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D46" s="43"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
@@ -15405,6 +15419,9 @@
       <c r="C47" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D47" s="43" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
@@ -15416,6 +15433,7 @@
       <c r="C48" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D48" s="43"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
@@ -15427,6 +15445,9 @@
       <c r="C49" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D49" s="43" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
@@ -15438,6 +15459,7 @@
       <c r="C50" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D50" s="43"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
@@ -15493,7 +15515,7 @@
       <c r="C55" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="D55" s="43" t="s">
         <v>203</v>
       </c>
     </row>
@@ -15504,9 +15526,10 @@
       <c r="B56" t="s">
         <v>165</v>
       </c>
-      <c r="C56" s="39" t="s">
+      <c r="C56" s="37" t="s">
         <v>190</v>
       </c>
+      <c r="D56" s="43"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1">
@@ -15515,10 +15538,10 @@
       <c r="B57" t="s">
         <v>166</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C57" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="D57" s="41" t="s">
+      <c r="D57" s="43" t="s">
         <v>202</v>
       </c>
     </row>
@@ -15529,9 +15552,10 @@
       <c r="B58" t="s">
         <v>167</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="37" t="s">
         <v>190</v>
       </c>
+      <c r="D58" s="43"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
@@ -15732,11 +15756,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -15751,8 +15785,10 @@
     <hyperlink ref="D45" r:id="rId10"/>
     <hyperlink ref="D55" r:id="rId11"/>
     <hyperlink ref="D57" r:id="rId12"/>
+    <hyperlink ref="D47:D48" r:id="rId13" display="C780_PT15_FW_Code_Inspection_Plan_nvm_CAREL.xlsx"/>
+    <hyperlink ref="D49:D50" r:id="rId14" display="C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
see inspection plan check files
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="3600" windowWidth="46296" windowHeight="13296" activeTab="2"/>
+    <workbookView xWindow="396" yWindow="600" windowWidth="19824" windowHeight="7200" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
     <sheet name="Files_Check_List" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="215">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -463,9 +468,6 @@
     <t>Led_Manager_IS.h</t>
   </si>
   <si>
-    <t>lista.txt</t>
-  </si>
-  <si>
     <t>main_CAREL.c</t>
   </si>
   <si>
@@ -575,9 +577,6 @@
   </si>
   <si>
     <t>test_hw_CAREL.h</t>
-  </si>
-  <si>
-    <t>tinycbor</t>
   </si>
   <si>
     <t>types.h</t>
@@ -615,9 +614,6 @@
     <t>Bilato</t>
   </si>
   <si>
-    <t>Cellini</t>
-  </si>
-  <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_Binary_model.xlsx</t>
   </si>
   <si>
@@ -630,34 +626,67 @@
     <t>C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx</t>
   </si>
   <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_File_System_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_gme_types_h.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_ https_client_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_https_client_IS</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_http_server_IS.xlsx</t>
+  </si>
+  <si>
+    <t>Zero Warning</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_ ota_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_polling_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_polling_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_MQTT_Interface_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_MQTT_Interface_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_Modbus_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_main_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_main_CAREL.xlsx</t>
+  </si>
+  <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_Led_manager.xlsx</t>
   </si>
   <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_main_CAREL.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_main_IS.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_Modbus_IS.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_MQTT_Interface_CAREL.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_polling_IS.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_polling_CAREL.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_CAREL.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx</t>
-  </si>
-  <si>
-    <t>C780_PT15_FW_Code_Inspection_Plan_ota_CAREL.xlsx</t>
+    <t>tinycbor [FOLDER]</t>
   </si>
 </sst>
 </file>
@@ -707,7 +736,7 @@
       <name val="SimSun"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,8 +749,14 @@
         <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1054,12 +1089,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1107,11 +1213,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1123,13 +1239,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,7 +1316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1227,7 +1351,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,15 +1582,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="39"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6605,13 +6729,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14848,11 +14972,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14861,943 +14985,1170 @@
     <col min="2" max="2" width="27.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="74.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A1" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="D2" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="37">
+        <v>2</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="37">
+        <v>3</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="37">
+        <v>4</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="37">
+        <v>5</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="37">
+        <v>6</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="37">
+        <v>7</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="34">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="34">
+        <v>9</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="34">
+        <v>10</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="34">
+        <v>11</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="34">
+        <v>12</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="34">
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="34">
+        <v>14</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="34">
+        <v>15</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="34">
+        <v>16</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="34">
+        <v>17</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="34">
+        <v>18</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="34">
+        <v>19</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="34">
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="34">
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="34">
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="34">
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="39">
+        <v>24</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="58"/>
+      <c r="E25" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="37">
+        <v>25</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="35" customFormat="1">
+      <c r="A27" s="41">
+        <v>26</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="37">
+        <v>27</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="44"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="44"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="43"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="43"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1">
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="37">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1">
+      <c r="C29" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="37"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="37">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1">
+      <c r="C30" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="E30" s="37"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="37">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1">
+      <c r="C31" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31" s="37"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="37">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" s="46"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1">
+      <c r="C32" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D32" s="63"/>
+      <c r="E32" s="37"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="37">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="37"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="37">
+        <v>33</v>
+      </c>
+      <c r="B34" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="37"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="37">
+        <v>34</v>
+      </c>
+      <c r="B35" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C35" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="37"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="37">
+        <v>35</v>
+      </c>
+      <c r="B36" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D35" s="45"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="35" customFormat="1">
+      <c r="A37" s="41">
+        <v>36</v>
+      </c>
+      <c r="B37" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D36" s="45" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="64"/>
+      <c r="E37" s="41"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="37">
+        <v>37</v>
+      </c>
+      <c r="B38" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="45"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C38" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="37"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="37">
+        <v>38</v>
+      </c>
+      <c r="B39" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C39" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="60"/>
+      <c r="E39" s="37"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="37">
+        <v>39</v>
+      </c>
+      <c r="B40" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="61"/>
+      <c r="E40" s="37"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="37">
+        <v>40</v>
+      </c>
+      <c r="B41" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C41" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="37">
+        <v>41</v>
+      </c>
+      <c r="B42" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D41" s="45" t="s">
+      <c r="C42" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D42" s="64"/>
+      <c r="E42" s="37"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="37">
+        <v>42</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="64" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="37" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="45"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" s="37">
+        <v>43</v>
+      </c>
+      <c r="B44" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D43" s="45" t="s">
+      <c r="C44" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="64"/>
+      <c r="E44" s="37"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="37">
+        <v>44</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="37">
+        <v>45</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D46" s="55"/>
+      <c r="E46" s="37"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="37">
+        <v>46</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D47" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47" s="37"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="37">
+        <v>47</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="55"/>
+      <c r="E48" s="37"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="37">
+        <v>48</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" s="37"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="37">
+        <v>49</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" s="55"/>
+      <c r="E50" s="37"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="37">
+        <v>50</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D51" s="59"/>
+      <c r="E51" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="13.8" customHeight="1">
+      <c r="A52" s="37">
+        <v>51</v>
+      </c>
+      <c r="B52" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" s="55"/>
+      <c r="E52" s="37"/>
+    </row>
+    <row r="53" spans="1:5" s="35" customFormat="1">
+      <c r="A53" s="41">
+        <v>52</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D53" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="E53" s="56" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D44" s="45"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="45"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="45" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54" s="37">
+        <v>53</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D54" s="62"/>
+      <c r="E54" s="56"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="37">
+        <v>54</v>
+      </c>
+      <c r="B55" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="59" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D48" s="45"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="45" t="s">
+      <c r="E55" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="37">
+        <v>55</v>
+      </c>
+      <c r="B56" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D56" s="55"/>
+      <c r="E56" s="37"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="37">
+        <v>56</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" s="59" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>159</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D50" s="45"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>160</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D51" s="45" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>161</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D52" s="45"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" s="45"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="E57" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="37">
+        <v>57</v>
+      </c>
+      <c r="B58" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C57" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C58" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="55"/>
+      <c r="E58" s="37"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="37">
+        <v>58</v>
+      </c>
+      <c r="B59" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="C58" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D58" s="45"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C59" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="54"/>
+      <c r="E59" s="37"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="37">
+        <v>59</v>
+      </c>
+      <c r="B60" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C60" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" s="54"/>
+      <c r="E60" s="37"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="37">
+        <v>60</v>
+      </c>
+      <c r="B61" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C61" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="54"/>
+      <c r="E61" s="37"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="37">
+        <v>61</v>
+      </c>
+      <c r="B62" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C62" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="54"/>
+      <c r="E62" s="37"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="37">
+        <v>62</v>
+      </c>
+      <c r="B63" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C63" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="54"/>
+      <c r="E63" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="37">
+        <v>63</v>
+      </c>
+      <c r="B64" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C64" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="54"/>
+      <c r="E64" s="37"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="37">
+        <v>64</v>
+      </c>
+      <c r="B65" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C65" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" s="54"/>
+      <c r="E65" s="37"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="37">
+        <v>65</v>
+      </c>
+      <c r="B66" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C66" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="54"/>
+      <c r="E66" s="37"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="37">
+        <v>66</v>
+      </c>
+      <c r="B67" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C67" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67" s="54"/>
+      <c r="E67" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="37">
+        <v>67</v>
+      </c>
+      <c r="B68" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C68" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="54"/>
+      <c r="E68" s="37"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="37">
+        <v>68</v>
+      </c>
+      <c r="B69" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C69" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D69" s="54"/>
+      <c r="E69" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="37">
+        <v>69</v>
+      </c>
+      <c r="B70" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C70" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" s="54"/>
+      <c r="E70" s="37"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="37">
+        <v>70</v>
+      </c>
+      <c r="B71" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" s="38"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="37">
+        <v>71</v>
+      </c>
+      <c r="B72" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C72" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="37">
+        <v>72</v>
+      </c>
+      <c r="B73" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1">
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C73" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D73" s="54"/>
+      <c r="E73" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="37">
+        <v>73</v>
+      </c>
+      <c r="B74" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C74" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D74" s="54"/>
+      <c r="E74" s="37"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="37">
+        <v>74</v>
+      </c>
+      <c r="B75" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C75" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="54"/>
+      <c r="E75" s="37"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="37">
+        <v>75</v>
+      </c>
+      <c r="B76" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>184</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="C76" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D76" s="54"/>
+      <c r="E76" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
+  <mergeCells count="32">
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D47:D48"/>
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D39:D40"/>
     <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D36:D37"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D5" r:id="rId2"/>
     <hyperlink ref="D10:D11" r:id="rId3" display="C780_PT15_FW_Code_Inspection_Plan_data_types_CAREL_IS.xlsx"/>
     <hyperlink ref="D12:D13" r:id="rId4" display="C780_PT15_FW_Code_Inspection_Plan_File_System_CAREL.xlsx"/>
-    <hyperlink ref="D31" r:id="rId5"/>
-    <hyperlink ref="D34" r:id="rId6"/>
-    <hyperlink ref="D36" r:id="rId7"/>
-    <hyperlink ref="D41" r:id="rId8"/>
-    <hyperlink ref="D43" r:id="rId9"/>
-    <hyperlink ref="D45" r:id="rId10"/>
-    <hyperlink ref="D55" r:id="rId11"/>
-    <hyperlink ref="D57" r:id="rId12"/>
+    <hyperlink ref="D14:D15" r:id="rId5" display="C780_PT15_FW_Code_Inspection_Plan_File_System_IS.xlsx"/>
+    <hyperlink ref="D17" r:id="rId6"/>
+    <hyperlink ref="D18:D19" r:id="rId7" display="C780_PT15_FW_Code_Inspection_Plan_ https_client_CAREL.xlsx"/>
+    <hyperlink ref="D20:D21" r:id="rId8" display="C780_PT15_FW_Code_Inspection_Plan_ https_client_CAREL.xlsx"/>
+    <hyperlink ref="D22:D23" r:id="rId9" display="C780_PT15_FW_Code_Inspection_Plan_https_client_IS"/>
+    <hyperlink ref="D26:D27" r:id="rId10" display="C780_PT15_FW_Code_Inspection_Plan_http_server_IS.xlsx"/>
+    <hyperlink ref="D45:D46" r:id="rId11" display="C780_PT15_FW_Code_Inspection_Plan_MQTT_Interface_IS.xlsx"/>
+    <hyperlink ref="D49:D50" r:id="rId12" display="C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx"/>
     <hyperlink ref="D47:D48" r:id="rId13" display="C780_PT15_FW_Code_Inspection_Plan_nvm_CAREL.xlsx"/>
-    <hyperlink ref="D49:D50" r:id="rId14" display="C780_PT15_FW_Code_Inspection_Plan_nvm_IS.xlsx"/>
-    <hyperlink ref="D51:D52" r:id="rId15" display="C780_PT15_FW_Code_Inspection_Plan_ota_CAREL.xlsx"/>
+    <hyperlink ref="D57:D58" r:id="rId14" display="C780_PT15_FW_Code_Inspection_Plan_polling_IS.xlsx"/>
+    <hyperlink ref="D55:D56" r:id="rId15" display="C780_PT15_FW_Code_Inspection_Plan_polling_CAREL.xlsx"/>
+    <hyperlink ref="D53:D54" r:id="rId16" display="Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_ ota_IS.xlsx"/>
+    <hyperlink ref="D31" r:id="rId17"/>
+    <hyperlink ref="D34" r:id="rId18"/>
+    <hyperlink ref="D36" r:id="rId19"/>
+    <hyperlink ref="D41" r:id="rId20"/>
+    <hyperlink ref="D43" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added result of CPPCheck
</commit_message>
<xml_diff>
--- a/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
+++ b/Test/C780_PT15_FW_Code_Inspection_Plan.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2952" yWindow="5892" windowWidth="57804" windowHeight="16452" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="1848" yWindow="3600" windowWidth="46296" windowHeight="13176" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
     <sheet name="Files_Check_List" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="228">
   <si>
     <t>Code Inspection rules</t>
   </si>
@@ -694,6 +699,30 @@
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_utilities_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>CPPCheck</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>rework necessary</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_radio.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_RTC_IS.xlsx</t>
+  </si>
+  <si>
+    <t>C780_PT15_FW_Code_Inspection_Plan_SoftWDT.xlsx</t>
+  </si>
+  <si>
+    <t>Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_sys_CAREL.xlsx</t>
+  </si>
+  <si>
+    <t>rework necessary search TODO CPPCHECK</t>
   </si>
   <si>
     <t>C780_PT15_FW_Code_Inspection_Plan_wifi.xlsx</t>
@@ -746,7 +775,7 @@
       <name val="SimSun"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,8 +794,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1159,9 +1194,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1170,12 +1203,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1237,7 +1303,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1249,22 +1322,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -1326,7 +1402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1361,7 +1437,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1592,15 +1668,15 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="56"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
@@ -6739,13 +6815,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A2" s="34"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" ht="13.65" customHeight="1" thickBot="1">
       <c r="A3" s="34"/>
@@ -14982,11 +15058,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75:D76"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14996,9 +15072,10 @@
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="74.109375" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.4" thickBot="1">
+    <row r="1" spans="1:7" ht="29.4" thickBot="1">
       <c r="A1" s="44" t="s">
         <v>187</v>
       </c>
@@ -15011,11 +15088,14 @@
       <c r="D1" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="53" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="43">
         <v>1</v>
       </c>
@@ -15025,14 +15105,17 @@
       <c r="C2" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="50" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -15042,12 +15125,13 @@
       <c r="C3" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="37" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -15058,11 +15142,12 @@
         <v>189</v>
       </c>
       <c r="D4" s="37"/>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -15072,14 +15157,18 @@
       <c r="C5" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="64" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="G5" s="74"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -15089,12 +15178,13 @@
       <c r="C6" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="37" t="s">
+      <c r="D6" s="65"/>
+      <c r="E6" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -15107,9 +15197,10 @@
       <c r="D7" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="51"/>
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="37">
         <v>7</v>
       </c>
@@ -15120,9 +15211,10 @@
         <v>189</v>
       </c>
       <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="51"/>
+      <c r="F8" s="47"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="34">
         <v>8</v>
       </c>
@@ -15133,9 +15225,10 @@
         <v>189</v>
       </c>
       <c r="D9" s="34"/>
-      <c r="E9" s="37"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="51"/>
+      <c r="F9" s="47"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="34">
         <v>9</v>
       </c>
@@ -15145,14 +15238,15 @@
       <c r="C10" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="64" t="s">
         <v>192</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -15162,12 +15256,13 @@
       <c r="C11" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="37" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="34">
         <v>11</v>
       </c>
@@ -15177,14 +15272,17 @@
       <c r="C12" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="34">
         <v>12</v>
       </c>
@@ -15194,12 +15292,13 @@
       <c r="C13" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="37" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="61"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -15209,14 +15308,17 @@
       <c r="C14" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="34">
         <v>14</v>
       </c>
@@ -15226,12 +15328,13 @@
       <c r="C15" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="37" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="61"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="34">
         <v>15</v>
       </c>
@@ -15242,11 +15345,12 @@
         <v>189</v>
       </c>
       <c r="D16" s="34"/>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="47"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="34">
         <v>16</v>
       </c>
@@ -15259,11 +15363,12 @@
       <c r="D17" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="47"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="34">
         <v>17</v>
       </c>
@@ -15273,14 +15378,17 @@
       <c r="C18" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="60" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="34">
         <v>18</v>
       </c>
@@ -15290,12 +15398,13 @@
       <c r="C19" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="37" t="s">
+      <c r="D19" s="64"/>
+      <c r="E19" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="61"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="34">
         <v>19</v>
       </c>
@@ -15305,14 +15414,17 @@
       <c r="C20" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="64" t="s">
         <v>196</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="34">
         <v>20</v>
       </c>
@@ -15322,12 +15434,13 @@
       <c r="C21" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="64"/>
+      <c r="E21" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="61"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="34">
         <v>21</v>
       </c>
@@ -15337,14 +15450,18 @@
       <c r="C22" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" s="74"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="34">
         <v>22</v>
       </c>
@@ -15354,12 +15471,13 @@
       <c r="C23" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="37" t="s">
+      <c r="D23" s="64"/>
+      <c r="E23" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="63"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="34">
         <v>23</v>
       </c>
@@ -15369,12 +15487,15 @@
       <c r="C24" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="37" t="s">
+      <c r="D24" s="69"/>
+      <c r="E24" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="39">
         <v>24</v>
       </c>
@@ -15384,12 +15505,13 @@
       <c r="C25" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="37" t="s">
+      <c r="D25" s="70"/>
+      <c r="E25" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="61"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="37">
         <v>25</v>
       </c>
@@ -15399,14 +15521,15 @@
       <c r="C26" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="35" customFormat="1">
+      <c r="F26" s="60"/>
+    </row>
+    <row r="27" spans="1:7" s="35" customFormat="1">
       <c r="A27" s="41">
         <v>26</v>
       </c>
@@ -15416,12 +15539,13 @@
       <c r="C27" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="41" t="s">
+      <c r="D27" s="69"/>
+      <c r="E27" s="52" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="61"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="37">
         <v>27</v>
       </c>
@@ -15432,9 +15556,10 @@
         <v>188</v>
       </c>
       <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="E28" s="51"/>
+      <c r="F28" s="47"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="37">
         <v>28</v>
       </c>
@@ -15445,9 +15570,10 @@
         <v>188</v>
       </c>
       <c r="D29" s="42"/>
-      <c r="E29" s="37"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="51"/>
+      <c r="F29" s="47"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="37">
         <v>29</v>
       </c>
@@ -15460,9 +15586,10 @@
       <c r="D30" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="E30" s="37"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="51"/>
+      <c r="F30" s="47"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="37">
         <v>30</v>
       </c>
@@ -15472,12 +15599,15 @@
       <c r="C31" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="68" t="s">
         <v>213</v>
       </c>
-      <c r="E31" s="37"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31" s="51"/>
+      <c r="F31" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="37">
         <v>31</v>
       </c>
@@ -15487,19 +15617,21 @@
       <c r="C32" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="37"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32" s="68"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="61"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="37">
         <v>32</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" s="37"/>
       <c r="D33" s="42"/>
-      <c r="E33" s="37"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33" s="51"/>
+      <c r="F33" s="47"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="37">
         <v>33</v>
       </c>
@@ -15509,12 +15641,15 @@
       <c r="C34" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E34" s="37"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="E34" s="51"/>
+      <c r="F34" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="37">
         <v>34</v>
       </c>
@@ -15524,10 +15659,11 @@
       <c r="C35" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="57"/>
-      <c r="E35" s="37"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="D35" s="67"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="63"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="37">
         <v>35</v>
       </c>
@@ -15537,14 +15673,15 @@
       <c r="C36" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="E36" s="37" t="s">
+      <c r="E36" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" s="35" customFormat="1">
+      <c r="F36" s="60"/>
+    </row>
+    <row r="37" spans="1:7" s="35" customFormat="1">
       <c r="A37" s="41">
         <v>36</v>
       </c>
@@ -15554,10 +15691,11 @@
       <c r="C37" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="D37" s="67"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="61"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="37">
         <v>37</v>
       </c>
@@ -15568,9 +15706,10 @@
         <v>188</v>
       </c>
       <c r="D38" s="42"/>
-      <c r="E38" s="37"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38" s="51"/>
+      <c r="F38" s="47"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="37">
         <v>38</v>
       </c>
@@ -15580,10 +15719,13 @@
       <c r="C39" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D39" s="63"/>
-      <c r="E39" s="37"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="D39" s="60"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="37">
         <v>39</v>
       </c>
@@ -15593,10 +15735,11 @@
       <c r="C40" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="37"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D40" s="61"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="61"/>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="37">
         <v>40</v>
       </c>
@@ -15606,14 +15749,18 @@
       <c r="C41" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D41" s="57" t="s">
+      <c r="D41" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E41" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G41" s="74"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="37">
         <v>41</v>
       </c>
@@ -15623,10 +15770,11 @@
       <c r="C42" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="37"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="D42" s="67"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="63"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="37">
         <v>42</v>
       </c>
@@ -15636,14 +15784,18 @@
       <c r="C43" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="57" t="s">
+      <c r="D43" s="67" t="s">
         <v>209</v>
       </c>
-      <c r="E43" s="37" t="s">
+      <c r="E43" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" s="74"/>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="37">
         <v>43</v>
       </c>
@@ -15653,10 +15805,11 @@
       <c r="C44" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D44" s="57"/>
-      <c r="E44" s="37"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="D44" s="67"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="63"/>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="37">
         <v>44</v>
       </c>
@@ -15666,14 +15819,17 @@
       <c r="C45" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="71" t="s">
         <v>208</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E45" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="37">
         <v>45</v>
       </c>
@@ -15683,10 +15839,11 @@
       <c r="C46" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D46" s="55"/>
-      <c r="E46" s="37"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="D46" s="66"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="61"/>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="37">
         <v>46</v>
       </c>
@@ -15696,12 +15853,15 @@
       <c r="C47" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D47" s="54" t="s">
+      <c r="D47" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="E47" s="37"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="E47" s="51"/>
+      <c r="F47" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="37">
         <v>47</v>
       </c>
@@ -15711,10 +15871,11 @@
       <c r="C48" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D48" s="55"/>
-      <c r="E48" s="37"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="D48" s="66"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="61"/>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="37">
         <v>48</v>
       </c>
@@ -15724,12 +15885,15 @@
       <c r="C49" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D49" s="54" t="s">
+      <c r="D49" s="71" t="s">
         <v>207</v>
       </c>
-      <c r="E49" s="37"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="E49" s="51"/>
+      <c r="F49" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="37">
         <v>49</v>
       </c>
@@ -15739,10 +15903,11 @@
       <c r="C50" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="55"/>
-      <c r="E50" s="37"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="D50" s="66"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="63"/>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="37">
         <v>50</v>
       </c>
@@ -15752,14 +15917,18 @@
       <c r="C51" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D51" s="54" t="s">
+      <c r="D51" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E51" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="13.8" customHeight="1">
+      <c r="F51" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G51" s="74"/>
+    </row>
+    <row r="52" spans="1:7" ht="13.8" customHeight="1">
       <c r="A52" s="37">
         <v>51</v>
       </c>
@@ -15769,10 +15938,11 @@
       <c r="C52" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="55"/>
-      <c r="E52" s="37"/>
-    </row>
-    <row r="53" spans="1:5" s="35" customFormat="1">
+      <c r="D52" s="66"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="63"/>
+    </row>
+    <row r="53" spans="1:7" s="35" customFormat="1">
       <c r="A53" s="41">
         <v>52</v>
       </c>
@@ -15782,14 +15952,17 @@
       <c r="C53" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="D53" s="58" t="s">
+      <c r="D53" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="E53" s="60" t="s">
+      <c r="E53" s="73" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="37">
         <v>53</v>
       </c>
@@ -15799,10 +15972,11 @@
       <c r="C54" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D54" s="59"/>
-      <c r="E54" s="60"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="D54" s="72"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="61"/>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="37">
         <v>54</v>
       </c>
@@ -15812,14 +15986,18 @@
       <c r="C55" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="54" t="s">
+      <c r="D55" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="E55" s="37" t="s">
+      <c r="E55" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G55" s="74"/>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="37">
         <v>55</v>
       </c>
@@ -15829,10 +16007,11 @@
       <c r="C56" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="55"/>
-      <c r="E56" s="37"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="D56" s="66"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="63"/>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="37">
         <v>56</v>
       </c>
@@ -15842,14 +16021,17 @@
       <c r="C57" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D57" s="54" t="s">
+      <c r="D57" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="E57" s="37" t="s">
+      <c r="E57" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="37">
         <v>57</v>
       </c>
@@ -15859,10 +16041,11 @@
       <c r="C58" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D58" s="55"/>
-      <c r="E58" s="37"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="D58" s="66"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="61"/>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="37">
         <v>58</v>
       </c>
@@ -15872,10 +16055,15 @@
       <c r="C59" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="D59" s="53"/>
-      <c r="E59" s="37"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="D59" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="E59" s="51"/>
+      <c r="F59" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="37">
         <v>59</v>
       </c>
@@ -15885,10 +16073,11 @@
       <c r="C60" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D60" s="53"/>
-      <c r="E60" s="37"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="D60" s="64"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="61"/>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="37">
         <v>60</v>
       </c>
@@ -15898,10 +16087,15 @@
       <c r="C61" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="53"/>
-      <c r="E61" s="37"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="D61" s="64" t="s">
+        <v>223</v>
+      </c>
+      <c r="E61" s="51"/>
+      <c r="F61" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="37">
         <v>61</v>
       </c>
@@ -15911,10 +16105,11 @@
       <c r="C62" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D62" s="53"/>
-      <c r="E62" s="37"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="D62" s="64"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="61"/>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="37">
         <v>62</v>
       </c>
@@ -15924,12 +16119,17 @@
       <c r="C63" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D63" s="53"/>
-      <c r="E63" s="37" t="s">
+      <c r="D63" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="E63" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="37">
         <v>63</v>
       </c>
@@ -15939,10 +16139,11 @@
       <c r="C64" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D64" s="53"/>
-      <c r="E64" s="37"/>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="D64" s="64"/>
+      <c r="E64" s="51"/>
+      <c r="F64" s="61"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="37">
         <v>64</v>
       </c>
@@ -15952,10 +16153,15 @@
       <c r="C65" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D65" s="53"/>
-      <c r="E65" s="37"/>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="D65" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="E65" s="51"/>
+      <c r="F65" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="37">
         <v>65</v>
       </c>
@@ -15965,10 +16171,11 @@
       <c r="C66" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="D66" s="53"/>
-      <c r="E66" s="37"/>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="D66" s="64"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="61"/>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="37">
         <v>66</v>
       </c>
@@ -15978,14 +16185,17 @@
       <c r="C67" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D67" s="56" t="s">
+      <c r="D67" s="64" t="s">
         <v>216</v>
       </c>
-      <c r="E67" s="37" t="s">
+      <c r="E67" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="37">
         <v>67</v>
       </c>
@@ -15995,10 +16205,11 @@
       <c r="C68" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D68" s="56"/>
-      <c r="E68" s="37"/>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="D68" s="64"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="61"/>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="37">
         <v>68</v>
       </c>
@@ -16008,14 +16219,17 @@
       <c r="C69" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D69" s="56" t="s">
+      <c r="D69" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="E69" s="37" t="s">
+      <c r="E69" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="37">
         <v>69</v>
       </c>
@@ -16025,10 +16239,11 @@
       <c r="C70" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D70" s="56"/>
-      <c r="E70" s="37"/>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="D70" s="64"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="61"/>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="37">
         <v>70</v>
       </c>
@@ -16037,9 +16252,10 @@
       </c>
       <c r="C71" s="38"/>
       <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="E71" s="51"/>
+      <c r="F71" s="47"/>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="37">
         <v>71</v>
       </c>
@@ -16050,9 +16266,10 @@
         <v>188</v>
       </c>
       <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="E72" s="51"/>
+      <c r="F72" s="47"/>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="37">
         <v>72</v>
       </c>
@@ -16062,14 +16279,17 @@
       <c r="C73" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D73" s="56" t="s">
+      <c r="D73" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="E73" s="37" t="s">
+      <c r="E73" s="51" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" s="60" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="37">
         <v>73</v>
       </c>
@@ -16079,10 +16299,11 @@
       <c r="C74" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D74" s="56"/>
-      <c r="E74" s="37"/>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="D74" s="64"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="61"/>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="37">
         <v>74</v>
       </c>
@@ -16092,12 +16313,15 @@
       <c r="C75" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D75" s="56" t="s">
-        <v>219</v>
-      </c>
-      <c r="E75" s="37"/>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="D75" s="64" t="s">
+        <v>227</v>
+      </c>
+      <c r="E75" s="51"/>
+      <c r="F75" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="37">
         <v>75</v>
       </c>
@@ -16107,32 +16331,12 @@
       <c r="C76" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D76" s="56"/>
-      <c r="E76" s="37"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D49:D50"/>
+  <mergeCells count="60">
     <mergeCell ref="D75:D76"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="D63:D64"/>
@@ -16144,6 +16348,55 @@
     <mergeCell ref="D61:D62"/>
     <mergeCell ref="D55:D56"/>
     <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F67:F68"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -16170,10 +16423,14 @@
     <hyperlink ref="D51:D52" r:id="rId22" display="C780_PT15_FW_Code_Inspection_Plan_ota_CAREL.xlsx"/>
     <hyperlink ref="D67:D68" r:id="rId23" display="C780_PT15_FW_Code_Inspection_Plan_sys_IS.xlsx"/>
     <hyperlink ref="D69:D70" r:id="rId24" display="C780_PT15_FW_Code_Inspection_Plan_test_hw_CAREL.xlsx"/>
-    <hyperlink ref="D73:D74" r:id="rId25" display="C780_PT15_FW_Code_Inspection_Plan_utilities_CAREL.xlsx"/>
-    <hyperlink ref="D75:D76" r:id="rId26" display="C780_PT15_FW_Code_Inspection_Plan_wifi.xlsx"/>
+    <hyperlink ref="D59:D60" r:id="rId25" display="Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_radio.xlsx"/>
+    <hyperlink ref="D61:D62" r:id="rId26" display="Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_RTC_IS.xlsx"/>
+    <hyperlink ref="D63:D64" r:id="rId27" display="Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_SoftWDT.xlsx"/>
+    <hyperlink ref="D65:D66" r:id="rId28" display="Code_Inspection_Plan_Results\C780_PT15_FW_Code_Inspection_Plan_sys_CAREL.xlsx"/>
+    <hyperlink ref="D73:D74" r:id="rId29" display="C780_PT15_FW_Code_Inspection_Plan_utilities_CAREL.xlsx"/>
+    <hyperlink ref="D75:D76" r:id="rId30" display="C780_PT15_FW_Code_Inspection_Plan_wifi.xlsx"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>